<commit_message>
progress on adding instream flow limits to SWBM
</commit_message>
<xml_diff>
--- a/mgmt_scenarios_2020_summer_notes.xlsx
+++ b/mgmt_scenarios_2020_summer_notes.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E5F30-9CFF-41A0-8FF4-869079593322}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A46A46-CA60-4F8D-BA92-8C22D7F157FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fortran notes" sheetId="1" r:id="rId1"/>
+    <sheet name="Data dictionary - values" sheetId="2" r:id="rId2"/>
+    <sheet name="Data dictionary - column names" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>Filename</t>
   </si>
@@ -29,6 +31,99 @@
   </si>
   <si>
     <t>What does "write(*, …)" mean? Specifically, does the * mean the terminal?</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>SWBM field polygons</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>subwn</t>
+  </si>
+  <si>
+    <t>Landuse</t>
+  </si>
+  <si>
+    <t>Irrigation</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>[float]</t>
+  </si>
+  <si>
+    <t>Area (m2)</t>
+  </si>
+  <si>
+    <t>Pasture</t>
+  </si>
+  <si>
+    <t>Subwatershed number. I.e., which tributary is this field closest to?</t>
+  </si>
+  <si>
+    <t>What is growing on this field/land area?</t>
+  </si>
+  <si>
+    <t>Flood</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Dry (Field has no water source)</t>
+  </si>
+  <si>
+    <t>Center pivot irrigation</t>
+  </si>
+  <si>
+    <t>Sub-irrigated</t>
+  </si>
+  <si>
+    <t>Water_Source</t>
+  </si>
+  <si>
+    <t>Wheel line irrigation</t>
+  </si>
+  <si>
+    <t>Groundwater</t>
+  </si>
+  <si>
+    <t>Mixed surface water and groundwater</t>
+  </si>
+  <si>
+    <t>Surface water</t>
+  </si>
+  <si>
+    <t>No ET/No Irrigation</t>
+  </si>
+  <si>
+    <t>Alfalfa/grain</t>
+  </si>
+  <si>
+    <t>Native Veg</t>
+  </si>
+  <si>
+    <t>What technology is used to irrigate this field/land area?</t>
+  </si>
+  <si>
+    <t>How large (in meters squared) is this field/land area?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is (are) the source(s) of water used </t>
+  </si>
+  <si>
+    <t>Map of the subwatersheds?</t>
   </si>
 </sst>
 </file>
@@ -346,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,6 +465,461 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E6526-0232-499F-8F51-2D01B3AFCB45}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>555</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>999</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A936B0-1380-41EC-BB80-5E7155A3CAA6}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clean up land use scenario terminology and start working on SVIHM.ets changes
</commit_message>
<xml_diff>
--- a/mgmt_scenarios_2020_summer_notes.xlsx
+++ b/mgmt_scenarios_2020_summer_notes.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A46A46-CA60-4F8D-BA92-8C22D7F157FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C73720-559C-4DEC-A295-D3DBA5687EDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fortran notes" sheetId="1" r:id="rId1"/>
-    <sheet name="Data dictionary - values" sheetId="2" r:id="rId2"/>
-    <sheet name="Data dictionary - column names" sheetId="3" r:id="rId3"/>
+    <sheet name="Scenario Inventory" sheetId="4" r:id="rId1"/>
+    <sheet name="Water year type options" sheetId="5" r:id="rId2"/>
+    <sheet name="Fortran notes" sheetId="1" r:id="rId3"/>
+    <sheet name="Data dictionary - values" sheetId="2" r:id="rId4"/>
+    <sheet name="Data dictionary - column names" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="127">
   <si>
     <t>Filename</t>
   </si>
@@ -124,13 +126,430 @@
   </si>
   <si>
     <t>Map of the subwatersheds?</t>
+  </si>
+  <si>
+    <t>Scenario Name</t>
+  </si>
+  <si>
+    <t>natveg_gwmixed_outside_adj_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natveg_outside_adj_0.05 </t>
+  </si>
+  <si>
+    <t>pvar_a_extr_95_07</t>
+  </si>
+  <si>
+    <t>pvar_a03</t>
+  </si>
+  <si>
+    <t>pvar_a05</t>
+  </si>
+  <si>
+    <t>pvar_a10</t>
+  </si>
+  <si>
+    <t>pvar_b70</t>
+  </si>
+  <si>
+    <t>pvar_b80</t>
+  </si>
+  <si>
+    <t>pvar_b90</t>
+  </si>
+  <si>
+    <t>pvar_c10</t>
+  </si>
+  <si>
+    <t>pvar_c20</t>
+  </si>
+  <si>
+    <t>pvar_c30</t>
+  </si>
+  <si>
+    <t>up2018</t>
+  </si>
+  <si>
+    <t>up2018_a</t>
+  </si>
+  <si>
+    <t>up2018_b</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>ILR</t>
+  </si>
+  <si>
+    <t>MAR_ILR</t>
+  </si>
+  <si>
+    <t>alf_irr_stop_jul10</t>
+  </si>
+  <si>
+    <t>alf_irr_stop_aug01</t>
+  </si>
+  <si>
+    <t>natveg_gwmixed_inside_adj_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natveg_inside_adj_0.05 </t>
+  </si>
+  <si>
+    <t>Scenario description</t>
+  </si>
+  <si>
+    <t>Crop water deficit (total, TAF/yr)</t>
+  </si>
+  <si>
+    <t>Combination of MAR and ILR scenarios (total acreage of XX,XXX).</t>
+  </si>
+  <si>
+    <t>Monthly flow value (avg, May-Nov)</t>
+  </si>
+  <si>
+    <t>Monthly flow change (avg, May-Nov)</t>
+  </si>
+  <si>
+    <t>Drydown days gained &gt; 10, 20, 30, 40 cfs (summer), FJ gauge</t>
+  </si>
+  <si>
+    <t>Reconnection days gained &gt; 10, 20, 30, 40 cfs, FJ gauge</t>
+  </si>
+  <si>
+    <t>Project acreage affected</t>
+  </si>
+  <si>
+    <t>Water budget by land use type</t>
+  </si>
+  <si>
+    <t>Deas report</t>
+  </si>
+  <si>
+    <t>4 categories</t>
+  </si>
+  <si>
+    <t>3 categories</t>
+  </si>
+  <si>
+    <t>Wet, Above Avg, Below Average, Dry</t>
+  </si>
+  <si>
+    <t>Wet, Average, Dry</t>
+  </si>
+  <si>
+    <t>Dividing lines</t>
+  </si>
+  <si>
+    <t>1 standard deviation (and mean, if 4 categories)</t>
+  </si>
+  <si>
+    <t>Quartiles</t>
+  </si>
+  <si>
+    <t>33% dividers</t>
+  </si>
+  <si>
+    <t>Do the river runoff and total (or oct-mar) precipitation water year types match each other well?</t>
+  </si>
+  <si>
+    <t>Decision: 3 categories, 33% dividers</t>
+  </si>
+  <si>
+    <t>Then, basis for water year type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two primary options: precipitation at weather stations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base water year type functionally? Based on stream connectivity at X date? </t>
+  </si>
+  <si>
+    <t>Can we predict May-September flows based on Oct-Apr flows+</t>
+  </si>
+  <si>
+    <t>Did Deas look at relationship between rainfall year type (oct-mar) and streamflow year type</t>
+  </si>
+  <si>
+    <t>Option 1) Tanaka-Deas 2009 approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oct-Mar valley floor rainfall. 13.5 inches breakpoint for dry years. 20 inches for breakpoint for avg and wet. </t>
+  </si>
+  <si>
+    <t>Prepare graphs of color-coded water year types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 2) more explicit </t>
+  </si>
+  <si>
+    <t>Divert surface water to over-irrigate fields and enhance groundwater recharge (XX,XXX acres) during the wet season (Dec-Mar) . Allow diversions from tributaries to continue as long as water is available (on a monthly volume basis).</t>
+  </si>
+  <si>
+    <t>Divert surface water to irrigate fields (XX,XXX acres) during the growing season (Apr-Jun or Jul) in lieu of pumping groundwater. Allow diversions from tributaries to continue as long as water is available (on a monthly volume basis).</t>
+  </si>
+  <si>
+    <t>Assumes unspecified irrigated crop change, reducing all irrigated acreage water demand by 20%.</t>
+  </si>
+  <si>
+    <t>Assumes unspecified irrigated crop change, reducing all irrigated acreage water demand by 10%.</t>
+  </si>
+  <si>
+    <t>flow_lims</t>
+  </si>
+  <si>
+    <t>Alfalfa irrigation ceases on Aug 1st of every growing season.</t>
+  </si>
+  <si>
+    <t>Alfalfa irrigation ceases on July 10th of every growing season.</t>
+  </si>
+  <si>
+    <t>irrig_0.8</t>
+  </si>
+  <si>
+    <t>irrig_0.9</t>
+  </si>
+  <si>
+    <t>Scenario ID</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>ilr</t>
+  </si>
+  <si>
+    <t>mar_ilr</t>
+  </si>
+  <si>
+    <t>80% Irrigation</t>
+  </si>
+  <si>
+    <t>90% Irrigation</t>
+  </si>
+  <si>
+    <t>Alfalfa irrigation schedule - July 10 end date</t>
+  </si>
+  <si>
+    <t>Alfalfa irrigation schedule - Aug 01 end date</t>
+  </si>
+  <si>
+    <t>Performance metrics</t>
+  </si>
+  <si>
+    <t>Scenario information</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turns off pumping for wells serving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all irrigated fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which have a "groundwater" or "mixed groundwater and surface water" irrigation source. Assumes that these fields, where pumping is turned off, revert to natural vegetation with a k_c value of 1.0. Assumes that all fields with 5% or more of their area overlapping with the adjudicated zone are "inside" the adjudicated zone. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turns off pumping for wells serving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all irrigated fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the SVIHM model. Assumes that these fields, where pumping is turned off, revert to natural vegetation with a k_c value of 1.0. Assumes that all fields with 5% or more of their area overlapping with the adjudicated zone are "inside" the adjudicated zone. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turns off pumping for wells serving fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the adjudicated zone, which have a "groundwater" or "mixed groundwater and surface water" irrigation source. Assumes that these fields, where pumping is turned off, revert to natural vegetation with a k_c value of 1.0. Assumes that all fields with 5% or more of their area overlapping with the adjudicated zone are "inside" the adjudicated zone. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turns off pumping for wells serving all fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the adjudicated zone. Assumes that these fields, where pumping is turned off, revert to natural vegetation with a k_c value of 1.0. Assumes that all fields with 5% or more of their area overlapping with the adjudicated zone are "inside" the adjudicated zone. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turns off pumping for wells serving fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the adjudicated zone, which have a "groundwater" or "mixed groundwater and surface water" irrigation source. Assumes that these fields, where pumping is turned off, revert to natural vegetation with a k_c value of 1.0. Assumes that all fields with 5% or more of their area overlapping with the adjudicated zone are "inside" the adjudicated zone. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turns off pumping for wells serving all fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the adjudicated zone. Assumes that these fields, where pumping is turned off, revert to natural vegetation with a k_c value of 1.0. Assumes that all fields with 5% or more of their area overlapping with the adjudicated zone are "inside" the adjudicated zone. </t>
+    </r>
+  </si>
+  <si>
+    <t>Scenario Type</t>
+  </si>
+  <si>
+    <t>Enhanced Recharge</t>
+  </si>
+  <si>
+    <t>Irrigation schedule change</t>
+  </si>
+  <si>
+    <t>Attribution - adjudicated area impacts</t>
+  </si>
+  <si>
+    <t>Reservoir</t>
+  </si>
+  <si>
+    <t>Small storage</t>
+  </si>
+  <si>
+    <t>Simulates a small reservoir on one tributary by withholding wet-season flow and releasing it during the dry season according to set operations rules.</t>
+  </si>
+  <si>
+    <t>Expanded MAR_ILR</t>
+  </si>
+  <si>
+    <t>Combination of MAR and ILR scenarios (total acreage of YY,YYY).</t>
+  </si>
+  <si>
+    <t>Crop change</t>
+  </si>
+  <si>
+    <t>Natural Vegetation Outside Adjudicated area (NVOA)</t>
+  </si>
+  <si>
+    <t>Natural Vegetation, on Groundwater- or Mixed-source fields, Outside Adjudicated area (NV-GWM-OA)</t>
+  </si>
+  <si>
+    <t>Natural Vegetation Inside Adjudicated area (NVIA)</t>
+  </si>
+  <si>
+    <t>Natural Vegetation, on Groundwater- or Mixed-source fields, Inside Adjudicated area (NV-GWM-IA)</t>
+  </si>
+  <si>
+    <t>Natural Vegetation (NV)</t>
+  </si>
+  <si>
+    <t>Natural Vegetation on all Groundwater- or Mixed-source fields (NV-GWM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +557,83 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -155,12 +641,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +1224,580 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C33109-873C-4229-8330-BBFF29839A47}">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="80.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="12" max="13" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" customWidth="1"/>
+    <col min="17" max="18" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
+    </row>
+    <row r="2" spans="1:18" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="21"/>
+    </row>
+    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="21"/>
+    </row>
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:18" ht="90" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:18" ht="90" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC670BE3-A5EA-40C0-9202-5CD5C90055F5}">
+  <dimension ref="A3:B30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -475,7 +1829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E6526-0232-499F-8F51-2D01B3AFCB45}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -839,7 +2193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A936B0-1380-41EC-BB80-5E7155A3CAA6}">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>